<commit_message>
Some classes are remastered
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/test.xlsx
+++ b/src/test/resources/xls/test.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fridges" sheetId="2" r:id="rId1"/>
-    <sheet name=" Phones" sheetId="3" r:id="rId2"/>
+    <sheet name="Phones" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Execute</t>
   </si>
@@ -131,9 +131,6 @@
     <t>1440x2880</t>
   </si>
   <si>
-    <t>S8</t>
-  </si>
-  <si>
     <t>J5</t>
   </si>
   <si>
@@ -159,6 +156,24 @@
   </si>
   <si>
     <t>Huawei</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Мобильные телефоны</t>
+  </si>
+  <si>
+    <t>Холодильники</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Смартфон Samsung Galaxy S8 Dual SIM 64GB (черный бриллиант) [G950FD]</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S8 Dual SIM 64GB (черный бриллиант) [G950FD]</t>
   </si>
 </sst>
 </file>
@@ -203,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,7 +230,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,21 +537,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,22 +563,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -564,22 +592,25 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -587,22 +618,25 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -610,22 +644,25 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -633,22 +670,25 @@
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -656,22 +696,25 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -679,25 +722,28 @@
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="C8" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="C10" s="2"/>
     </row>
   </sheetData>
@@ -708,22 +754,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" customWidth="1"/>
+    <col min="10" max="10" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,25 +782,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -757,25 +814,31 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="3">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2">
         <v>2017</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -783,25 +846,28 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3">
         <v>2015</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -809,25 +875,28 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="3">
+        <v>43</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="3">
         <v>2016</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -835,25 +904,28 @@
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="3">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="3">
         <v>2017</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -861,29 +933,33 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="3">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="3">
         <v>2017</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update of mappers requests
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/test.xlsx
+++ b/src/test/resources/xls/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Execute</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Samsung Galaxy S8 Dual SIM 64GB (черный бриллиант) [G950FD]</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -754,27 +757,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" customWidth="1"/>
-    <col min="10" max="10" width="68.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,179 +785,185 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>2017</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>2015</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>2016</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>2017</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>2017</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>

</xml_diff>